<commit_message>
CSV file and pandas library started
</commit_message>
<xml_diff>
--- a/Calender.xlsx
+++ b/Calender.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaya/Documents/-100daysofCode-Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{947918C8-CFF3-6743-AD48-A628FD306FF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E528EC-2BBB-BE46-A7EA-9FB80C41C61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14440" xr2:uid="{FF60FC64-C5C9-A748-B4F2-C6A8DA325619}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14420" xr2:uid="{FF60FC64-C5C9-A748-B4F2-C6A8DA325619}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">17 -OOP started -explained </t>
   </si>
@@ -43,6 +43,27 @@
   </si>
   <si>
     <t>done some turtle graphic 20</t>
+  </si>
+  <si>
+    <t>pandas 27</t>
+  </si>
+  <si>
+    <t>file handling26</t>
+  </si>
+  <si>
+    <t>21 turtle</t>
+  </si>
+  <si>
+    <t>22turtle</t>
+  </si>
+  <si>
+    <t>23turtle</t>
+  </si>
+  <si>
+    <t>24turtle</t>
+  </si>
+  <si>
+    <t>25turtle</t>
   </si>
 </sst>
 </file>
@@ -433,7 +454,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -507,26 +528,26 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>21</v>
-      </c>
-      <c r="B3" s="2">
-        <v>22</v>
-      </c>
-      <c r="C3" s="2">
-        <v>23</v>
-      </c>
-      <c r="D3" s="2">
-        <v>24</v>
-      </c>
-      <c r="E3" s="2">
-        <v>25</v>
-      </c>
-      <c r="F3" s="2">
-        <v>26</v>
-      </c>
-      <c r="G3" s="2">
-        <v>27</v>
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="H3" s="2">
         <v>28</v>

</xml_diff>

<commit_message>
list, dict comprehension with pandas done
</commit_message>
<xml_diff>
--- a/Calender.xlsx
+++ b/Calender.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaya/Documents/-100daysofCode-Python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71E528EC-2BBB-BE46-A7EA-9FB80C41C61C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E45918-5DB2-B847-BDBA-C00E5955680E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14420" xr2:uid="{FF60FC64-C5C9-A748-B4F2-C6A8DA325619}"/>
+    <workbookView xWindow="80" yWindow="500" windowWidth="25440" windowHeight="14400" xr2:uid="{FF60FC64-C5C9-A748-B4F2-C6A8DA325619}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t xml:space="preserve">17 -OOP started -explained </t>
   </si>
@@ -45,9 +45,6 @@
     <t>done some turtle graphic 20</t>
   </si>
   <si>
-    <t>pandas 27</t>
-  </si>
-  <si>
     <t>file handling26</t>
   </si>
   <si>
@@ -64,15 +61,28 @@
   </si>
   <si>
     <t>25turtle</t>
+  </si>
+  <si>
+    <t>pandas 27 US_state_game</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pandas again with list,dict comprehension28</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -122,20 +132,20 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -451,343 +461,337 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA6C7768-E854-5945-86EA-5995E91A184A}">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="21.5" defaultRowHeight="100" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="10" width="11.33203125" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="16384" width="21.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1">
+    <row r="1" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
         <v>1</v>
       </c>
-      <c r="B1" s="1">
+      <c r="B1" s="2">
         <v>2</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="2">
         <v>3</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="2">
         <v>4</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="2">
         <v>5</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1" s="2">
         <v>6</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G1" s="2">
         <v>7</v>
       </c>
-      <c r="H1" s="1">
+      <c r="H1" s="2">
         <v>8</v>
       </c>
-      <c r="I1" s="1">
+      <c r="I1" s="2">
         <v>9</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J1" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
+    <row r="2" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
         <v>11</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2">
         <v>12</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>13</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="2">
         <v>14</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="2">
         <v>15</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="2">
         <v>16</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="2">
         <v>19</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" s="2">
-        <v>28</v>
-      </c>
-      <c r="I3" s="2">
+      <c r="H3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="5">
         <v>29</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="5">
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
         <v>31</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="5">
         <v>32</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="5">
         <v>33</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="5">
         <v>34</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="5">
         <v>35</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="5">
         <v>36</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="5">
         <v>37</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="5">
         <v>38</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="5">
         <v>39</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="5">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
         <v>41</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="5">
         <v>42</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="5">
         <v>43</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="5">
         <v>44</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="5">
         <v>45</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="5">
         <v>46</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="5">
         <v>47</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="5">
         <v>48</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="5">
         <v>49</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="5">
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    <row r="6" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
         <v>51</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="5">
         <v>52</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="5">
         <v>53</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="5">
         <v>54</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="5">
         <v>55</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="5">
         <v>56</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="5">
         <v>57</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="5">
         <v>58</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="5">
         <v>59</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="5">
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="7" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
         <v>61</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="5">
         <v>62</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="5">
         <v>63</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="5">
         <v>64</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="5">
         <v>65</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="5">
         <v>66</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="5">
         <v>67</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="5">
         <v>68</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="5">
         <v>69</v>
       </c>
-      <c r="J7" s="2">
+      <c r="J7" s="5">
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    <row r="8" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
         <v>71</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="5">
         <v>72</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="5">
         <v>73</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="5">
         <v>74</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="5">
         <v>75</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="5">
         <v>76</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="5">
         <v>77</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="5">
         <v>78</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="5">
         <v>79</v>
       </c>
-      <c r="J8" s="2">
+      <c r="J8" s="5">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="9" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
         <v>81</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="5">
         <v>82</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="5">
         <v>83</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="5">
         <v>84</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="5">
         <v>85</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="5">
         <v>86</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="5">
         <v>87</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="5">
         <v>88</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="5">
         <v>89</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="5">
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="10" spans="1:10" ht="100" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
         <v>91</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="5">
         <v>92</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="5">
         <v>93</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="5">
         <v>94</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="5">
         <v>95</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="5">
         <v>96</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="5">
         <v>97</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="5">
         <v>98</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="5">
         <v>99</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="5">
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>